<commit_message>
Cambio de Nombre Generoca
</commit_message>
<xml_diff>
--- a/Disponibilidad.xlsx
+++ b/Disponibilidad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos Phyton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos Phyton\reporte_s_remoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -545,15 +545,9 @@
     <t>C_GASGRE_DNP30TCPIP.SV</t>
   </si>
   <si>
-    <t>C_GENERO_DNP.SV</t>
-  </si>
-  <si>
     <t>C_SCAR_D_RP5.SV</t>
   </si>
   <si>
-    <t>D_PERIPA_RP5.SV</t>
-  </si>
-  <si>
     <t>S_DOMING_RP5.SV</t>
   </si>
   <si>
@@ -978,6 +972,12 @@
   </si>
   <si>
     <t>YANACOCHA</t>
+  </si>
+  <si>
+    <t>C_GENEROCA</t>
+  </si>
+  <si>
+    <t>D_PERIPA</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1330,7 @@
         <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C1" t="s">
         <v>135</v>
@@ -1383,7 +1383,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1397,7 +1397,7 @@
         <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -1415,7 +1415,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
         <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1447,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
         <v>137</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -1479,7 +1479,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1493,7 +1493,7 @@
         <v>137</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
@@ -1511,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>139</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
@@ -1543,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>138</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1575,7 +1575,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>140</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>12</v>
@@ -1607,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1621,7 +1621,7 @@
         <v>137</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
@@ -1639,7 +1639,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1671,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
         <v>137</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
@@ -1703,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>17</v>
@@ -1767,7 +1767,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>137</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>18</v>
@@ -1799,7 +1799,7 @@
         <v>0.99850694462105083</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
         <v>142</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
@@ -1831,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>137</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>20</v>
@@ -1863,7 +1863,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>21</v>
@@ -1895,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1909,7 +1909,7 @@
         <v>143</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>22</v>
@@ -1927,7 +1927,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1941,7 +1941,7 @@
         <v>144</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>23</v>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1973,7 +1973,7 @@
         <v>145</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
@@ -1991,7 +1991,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2005,7 +2005,7 @@
         <v>137</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>25</v>
@@ -2023,7 +2023,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
         <v>142</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>26</v>
@@ -2055,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
         <v>138</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>27</v>
@@ -2087,7 +2087,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>0.999537037037037</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2133,7 +2133,7 @@
         <v>157</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>172</v>
+        <v>315</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>29</v>
@@ -2151,7 +2151,7 @@
         <v>0.73127314814814814</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2165,7 +2165,7 @@
         <v>142</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>30</v>
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
         <v>137</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>31</v>
@@ -2215,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2261,7 +2261,7 @@
         <v>137</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>33</v>
@@ -2279,7 +2279,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2293,7 +2293,7 @@
         <v>137</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>34</v>
@@ -2311,7 +2311,7 @@
         <v>4.1523776584201387E-2</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2325,7 +2325,7 @@
         <v>137</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>35</v>
@@ -2343,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2357,7 +2357,7 @@
         <v>142</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>36</v>
@@ -2375,7 +2375,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2389,7 +2389,7 @@
         <v>139</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>37</v>
@@ -2407,7 +2407,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2421,7 +2421,7 @@
         <v>148</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>38</v>
@@ -2439,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2453,7 +2453,7 @@
         <v>137</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>39</v>
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
         <v>138</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>40</v>
@@ -2503,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>149</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>41</v>
@@ -2535,7 +2535,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>149</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>42</v>
@@ -2567,7 +2567,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
         <v>137</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>43</v>
@@ -2599,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2613,7 +2613,7 @@
         <v>150</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>44</v>
@@ -2631,7 +2631,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2645,7 +2645,7 @@
         <v>151</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>45</v>
@@ -2663,7 +2663,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2677,7 +2677,7 @@
         <v>152</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>46</v>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2709,7 +2709,7 @@
         <v>137</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>47</v>
@@ -2727,7 +2727,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2741,7 +2741,7 @@
         <v>137</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>48</v>
@@ -2759,7 +2759,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2773,7 +2773,7 @@
         <v>137</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>49</v>
@@ -2791,7 +2791,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2802,7 +2802,7 @@
         <v>138</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>162</v>
@@ -2820,7 +2820,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2831,7 +2831,7 @@
         <v>152</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>163</v>
@@ -2849,7 +2849,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2860,10 +2860,10 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>50</v>
@@ -2881,7 +2881,7 @@
         <v>0.92869212962962966</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2892,10 +2892,10 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>51</v>
@@ -2913,7 +2913,7 @@
         <v>1.0000000120092323</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>137</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>52</v>
@@ -2945,7 +2945,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
         <v>137</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>53</v>
@@ -2974,7 +2974,7 @@
         <v>1</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -2988,7 +2988,7 @@
         <v>153</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>54</v>
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
@@ -3019,10 +3019,10 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>55</v>
@@ -3040,7 +3040,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3054,7 +3054,7 @@
         <v>138</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>56</v>
@@ -3072,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3080,10 +3080,10 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>57</v>
@@ -3101,7 +3101,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3112,10 +3112,10 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>58</v>
@@ -3133,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3147,7 +3147,7 @@
         <v>137</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>59</v>
@@ -3165,7 +3165,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3179,7 +3179,7 @@
         <v>137</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>60</v>
@@ -3197,7 +3197,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -3211,7 +3211,7 @@
         <v>138</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>61</v>
@@ -3229,7 +3229,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -3243,7 +3243,7 @@
         <v>137</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>62</v>
@@ -3261,7 +3261,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -3275,7 +3275,7 @@
         <v>137</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>63</v>
@@ -3293,7 +3293,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>137</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>164</v>
@@ -3325,7 +3325,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -3336,7 +3336,7 @@
         <v>137</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>64</v>
@@ -3354,7 +3354,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3368,7 +3368,7 @@
         <v>137</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>65</v>
@@ -3386,7 +3386,7 @@
         <v>0.99989583333333332</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3400,7 +3400,7 @@
         <v>138</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>66</v>
@@ -3418,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3432,7 +3432,7 @@
         <v>137</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>67</v>
@@ -3450,7 +3450,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3464,7 +3464,7 @@
         <v>137</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>68</v>
@@ -3482,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3493,7 +3493,7 @@
         <v>137</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>174</v>
+        <v>316</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>69</v>
@@ -3511,7 +3511,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3525,7 +3525,7 @@
         <v>137</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>70</v>
@@ -3543,7 +3543,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3557,7 +3557,7 @@
         <v>137</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>71</v>
@@ -3575,7 +3575,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3589,7 +3589,7 @@
         <v>154</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>72</v>
@@ -3607,7 +3607,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3621,7 +3621,7 @@
         <v>137</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>73</v>
@@ -3639,7 +3639,7 @@
         <v>0.95777777795438412</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3653,7 +3653,7 @@
         <v>137</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>74</v>
@@ -3671,7 +3671,7 @@
         <v>1</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3685,7 +3685,7 @@
         <v>138</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>75</v>
@@ -3703,7 +3703,7 @@
         <v>1</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3714,10 +3714,10 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>165</v>
@@ -3735,7 +3735,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3749,7 +3749,7 @@
         <v>137</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>76</v>
@@ -3767,7 +3767,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3781,7 +3781,7 @@
         <v>137</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>77</v>
@@ -3799,7 +3799,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3813,7 +3813,7 @@
         <v>155</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>78</v>
@@ -3831,7 +3831,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3845,7 +3845,7 @@
         <v>137</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>79</v>
@@ -3863,7 +3863,7 @@
         <v>1</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3877,7 +3877,7 @@
         <v>137</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>80</v>
@@ -3895,7 +3895,7 @@
         <v>1</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>138</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>81</v>
@@ -3927,7 +3927,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3941,7 +3941,7 @@
         <v>137</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>82</v>
@@ -3959,7 +3959,7 @@
         <v>1</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3970,7 +3970,7 @@
         <v>137</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>83</v>
@@ -3988,7 +3988,7 @@
         <v>1</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4002,7 +4002,7 @@
         <v>137</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>84</v>
@@ -4020,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4034,7 +4034,7 @@
         <v>138</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>85</v>
@@ -4052,7 +4052,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4066,7 +4066,7 @@
         <v>137</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>86</v>
@@ -4084,7 +4084,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -4098,7 +4098,7 @@
         <v>137</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>87</v>
@@ -4116,7 +4116,7 @@
         <v>0.96770833333333328</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -4130,7 +4130,7 @@
         <v>137</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>88</v>
@@ -4148,7 +4148,7 @@
         <v>1</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4162,7 +4162,7 @@
         <v>137</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>89</v>
@@ -4180,7 +4180,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -4194,7 +4194,7 @@
         <v>137</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>90</v>
@@ -4212,7 +4212,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4226,7 +4226,7 @@
         <v>137</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>91</v>
@@ -4244,7 +4244,7 @@
         <v>1</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4258,7 +4258,7 @@
         <v>138</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>92</v>
@@ -4276,7 +4276,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4290,7 +4290,7 @@
         <v>138</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>93</v>
@@ -4308,7 +4308,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4322,7 +4322,7 @@
         <v>137</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>94</v>
@@ -4340,7 +4340,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4354,7 +4354,7 @@
         <v>137</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>95</v>
@@ -4372,7 +4372,7 @@
         <v>1</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>137</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>96</v>
@@ -4404,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4418,7 +4418,7 @@
         <v>137</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>97</v>
@@ -4436,7 +4436,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4468,7 +4468,7 @@
         <v>1</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4482,7 +4482,7 @@
         <v>138</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>99</v>
@@ -4500,7 +4500,7 @@
         <v>1</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4514,7 +4514,7 @@
         <v>137</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>100</v>
@@ -4532,7 +4532,7 @@
         <v>1</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4546,7 +4546,7 @@
         <v>138</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>101</v>
@@ -4564,7 +4564,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4578,7 +4578,7 @@
         <v>138</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>102</v>
@@ -4596,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4610,7 +4610,7 @@
         <v>138</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>103</v>
@@ -4628,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,7 +4642,7 @@
         <v>137</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>104</v>
@@ -4660,7 +4660,7 @@
         <v>1</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4674,7 +4674,7 @@
         <v>137</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>105</v>
@@ -4692,7 +4692,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4706,7 +4706,7 @@
         <v>138</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>106</v>
@@ -4724,7 +4724,7 @@
         <v>1</v>
       </c>
       <c r="I107" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4738,7 +4738,7 @@
         <v>137</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>107</v>
@@ -4756,7 +4756,7 @@
         <v>1.0000000111262004</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4770,7 +4770,7 @@
         <v>137</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>108</v>
@@ -4788,7 +4788,7 @@
         <v>1</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4802,7 +4802,7 @@
         <v>137</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>109</v>
@@ -4820,7 +4820,7 @@
         <v>1</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4831,7 +4831,7 @@
         <v>137</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>110</v>
@@ -4849,7 +4849,7 @@
         <v>1</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4863,7 +4863,7 @@
         <v>137</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>111</v>
@@ -4881,7 +4881,7 @@
         <v>0.98182870370370368</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4895,7 +4895,7 @@
         <v>138</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>112</v>
@@ -4913,7 +4913,7 @@
         <v>1</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4927,7 +4927,7 @@
         <v>137</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>113</v>
@@ -4945,7 +4945,7 @@
         <v>0.99942129611968999</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4959,7 +4959,7 @@
         <v>137</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>114</v>
@@ -4977,7 +4977,7 @@
         <v>0</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
         <v>137</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>115</v>
@@ -5009,7 +5009,7 @@
         <v>1</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5023,7 +5023,7 @@
         <v>137</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>116</v>
@@ -5041,7 +5041,7 @@
         <v>1</v>
       </c>
       <c r="I117" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -5055,7 +5055,7 @@
         <v>137</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>117</v>
@@ -5073,7 +5073,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -5087,7 +5087,7 @@
         <v>137</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>118</v>
@@ -5105,7 +5105,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -5119,7 +5119,7 @@
         <v>137</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>119</v>
@@ -5137,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5148,7 +5148,7 @@
         <v>138</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>120</v>
@@ -5166,7 +5166,7 @@
         <v>1</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -5180,7 +5180,7 @@
         <v>137</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>121</v>
@@ -5198,7 +5198,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -5209,7 +5209,7 @@
         <v>138</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>166</v>
@@ -5227,7 +5227,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>137</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>122</v>
@@ -5259,7 +5259,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -5273,7 +5273,7 @@
         <v>161</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>123</v>
@@ -5291,7 +5291,7 @@
         <v>1</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -5302,7 +5302,7 @@
         <v>138</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>167</v>
@@ -5320,7 +5320,7 @@
         <v>1</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5331,7 +5331,7 @@
         <v>138</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>168</v>
@@ -5349,7 +5349,7 @@
         <v>1</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="128" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5360,7 +5360,7 @@
         <v>138</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>169</v>
@@ -5378,7 +5378,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I128" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -5392,7 +5392,7 @@
         <v>137</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>124</v>
@@ -5410,7 +5410,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5424,7 +5424,7 @@
         <v>137</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>125</v>
@@ -5442,7 +5442,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -5456,7 +5456,7 @@
         <v>137</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>126</v>
@@ -5474,7 +5474,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -5488,7 +5488,7 @@
         <v>137</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>127</v>
@@ -5502,7 +5502,7 @@
         <v>0.11377266848528826</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -5516,7 +5516,7 @@
         <v>138</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>128</v>
@@ -5530,7 +5530,7 @@
         <v>0.9999999998233936</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -5544,7 +5544,7 @@
         <v>138</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>129</v>
@@ -5558,7 +5558,7 @@
         <v>1</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5572,7 +5572,7 @@
         <v>138</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>130</v>
@@ -5586,7 +5586,7 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -5597,7 +5597,7 @@
         <v>138</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>131</v>
@@ -5611,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5625,7 +5625,7 @@
         <v>137</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>132</v>
@@ -5639,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5653,7 +5653,7 @@
         <v>137</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>133</v>
@@ -5667,7 +5667,7 @@
         <v>1</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -5681,7 +5681,7 @@
         <v>137</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>134</v>
@@ -5695,7 +5695,7 @@
         <v>1.0000000001766063</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>